<commit_message>
add tests and fixes part 1
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/sperfect_metadata_tables.xlsx
+++ b/tests/testthat/testdata/sperfect_metadata_tables.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10105"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lsibjb/Documents/Code/midar/tests/testthat/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5390913-AA4F-8E44-9A6A-632B7522E409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A837A478-9D21-4846-97FE-75BBDB1ACC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24380" yWindow="12600" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
+    <workbookView xWindow="24380" yWindow="12600" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{7A04E2C8-868F-5640-98CB-88D372530A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyses" sheetId="1" r:id="rId1"/>
     <sheet name="Features" sheetId="2" r:id="rId2"/>
     <sheet name="ISTDs" sheetId="3" r:id="rId3"/>
     <sheet name="RQCs" sheetId="4" r:id="rId4"/>
+    <sheet name="QCconc" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3149" uniqueCount="1080">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3171" uniqueCount="1089">
   <si>
     <t>analysis_id</t>
   </si>
@@ -3263,13 +3264,40 @@
   </si>
   <si>
     <t>analyzed_amount_unit</t>
+  </si>
+  <si>
+    <t>sample_id</t>
+  </si>
+  <si>
+    <t>concentration</t>
+  </si>
+  <si>
+    <t>concentration_unit</t>
+  </si>
+  <si>
+    <t>199_NIST_NIST04</t>
+  </si>
+  <si>
+    <t>S1P d18:1 [M&gt;60]</t>
+  </si>
+  <si>
+    <t>umol/L</t>
+  </si>
+  <si>
+    <t>198_LTR_LTR04</t>
+  </si>
+  <si>
+    <t>S1P d18:2 [M&gt;60]</t>
+  </si>
+  <si>
+    <t>S1P d18:0 [M&gt;60]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3403,6 +3431,19 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -3746,8 +3787,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -24918,7 +24961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE58D19-DFF1-D346-8279-6C7641F36845}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -25113,4 +25156,121 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17873042-8AD3-9A48-A30C-3D8A9EB1C366}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="A2:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>